<commit_message>
Updated pico pin info
</commit_message>
<xml_diff>
--- a/Design/PicoPinoutInfo.xlsx
+++ b/Design/PicoPinoutInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Documents\Arduino\RC_CAR\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Documents\pico-rc-car\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B800ADC-2999-4599-9581-A46AF3D6F202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A840704A-3EE9-4C03-A98A-C41BFCD4B4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="13356" windowHeight="12336" xr2:uid="{540CE9DB-4F91-4DA8-879B-A5CEB9C1B315}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{540CE9DB-4F91-4DA8-879B-A5CEB9C1B315}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -132,6 +132,27 @@
   </si>
   <si>
     <t>RUN</t>
+  </si>
+  <si>
+    <t>GP22</t>
+  </si>
+  <si>
+    <t>GP21</t>
+  </si>
+  <si>
+    <t>GP20</t>
+  </si>
+  <si>
+    <t>GP19</t>
+  </si>
+  <si>
+    <t>GP18</t>
+  </si>
+  <si>
+    <t>GP17</t>
+  </si>
+  <si>
+    <t>GP16</t>
   </si>
 </sst>
 </file>
@@ -554,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B7125D-1EE3-4F6F-B543-61BD7ED3092F}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,55 +757,49 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>20</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated all pinouts for the pico
</commit_message>
<xml_diff>
--- a/Design/PicoPinoutInfo.xlsx
+++ b/Design/PicoPinoutInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Documents\pico-rc-car\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A840704A-3EE9-4C03-A98A-C41BFCD4B4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B55E3E-DA52-4A40-8187-108EAF1E33EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{540CE9DB-4F91-4DA8-879B-A5CEB9C1B315}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="13140" windowHeight="12336" xr2:uid="{540CE9DB-4F91-4DA8-879B-A5CEB9C1B315}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -101,9 +101,6 @@
     <t>ESC</t>
   </si>
   <si>
-    <t>Controls the motor</t>
-  </si>
-  <si>
     <t>VBUS</t>
   </si>
   <si>
@@ -153,6 +150,66 @@
   </si>
   <si>
     <t>GP16</t>
+  </si>
+  <si>
+    <t>Servo</t>
+  </si>
+  <si>
+    <t>Used as ground for all components</t>
+  </si>
+  <si>
+    <t>Controls the motor of the car</t>
+  </si>
+  <si>
+    <t>Controls the steering of the car</t>
+  </si>
+  <si>
+    <t>Negative rail(right)</t>
+  </si>
+  <si>
+    <t>Positive rail(right)</t>
+  </si>
+  <si>
+    <t>Powers small components(ultrasonic sensor)</t>
+  </si>
+  <si>
+    <t>Step Motor IN4</t>
+  </si>
+  <si>
+    <t>Step Motor IN3</t>
+  </si>
+  <si>
+    <t>Step Motor IN2</t>
+  </si>
+  <si>
+    <t>Step Motor IN1</t>
+  </si>
+  <si>
+    <t>Allows the step motor to pivot back and forth</t>
+  </si>
+  <si>
+    <t>Ultrasonic Sensor Trigger</t>
+  </si>
+  <si>
+    <t>Ultrasonic Sensor Echo</t>
+  </si>
+  <si>
+    <t>Sends the ultrasonic pulse</t>
+  </si>
+  <si>
+    <t>Recieves the returning ultrasonic signal</t>
+  </si>
+  <si>
+    <t>LED indicator RED</t>
+  </si>
+  <si>
+    <t>LED indicator GREEN</t>
+  </si>
+  <si>
+    <t>If green light is lit up the area is clear</t>
+  </si>
+  <si>
+    <t>If red light is lit up the area is not clear</t>
   </si>
 </sst>
 </file>
@@ -211,16 +268,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>296175</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>108761</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533242</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>502038</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>129505</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>53407</xdr:rowOff>
+      <xdr:rowOff>138074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -243,7 +300,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6629242" y="481294"/>
+          <a:off x="6011175" y="565961"/>
           <a:ext cx="1425063" cy="3111180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -575,14 +632,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B7125D-1EE3-4F6F-B543-61BD7ED3092F}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -647,13 +705,25 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
       <c r="B13" t="s">
         <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -662,23 +732,47 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
       <c r="B18" t="s">
         <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -687,8 +781,14 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
       <c r="B20" t="s">
         <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -699,107 +799,131 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>22</v>
+      <c r="C22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ultrasonic Sensor pin change
</commit_message>
<xml_diff>
--- a/Design/PicoPinoutInfo.xlsx
+++ b/Design/PicoPinoutInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Documents\pico-rc-car\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B55E3E-DA52-4A40-8187-108EAF1E33EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E00CF7-69F8-4368-BBD6-C96FE0A0680F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="13140" windowHeight="12336" xr2:uid="{540CE9DB-4F91-4DA8-879B-A5CEB9C1B315}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{540CE9DB-4F91-4DA8-879B-A5CEB9C1B315}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -632,13 +632,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B7125D-1EE3-4F6F-B543-61BD7ED3092F}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" customWidth="1"/>
   </cols>
@@ -890,25 +890,13 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
       <c r="B37" t="s">
         <v>34</v>
       </c>
-      <c r="C37" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
       <c r="B38" t="s">
         <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -917,13 +905,25 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
       <c r="B40" t="s">
         <v>36</v>
       </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
       <c r="B41" t="s">
         <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed stop distance for ultrasonic from 30 to 50 cm, also attempted to implement an IR sensor for the rear(having issues)
</commit_message>
<xml_diff>
--- a/Design/PicoPinoutInfo.xlsx
+++ b/Design/PicoPinoutInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Documents\pico-rc-car\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E00CF7-69F8-4368-BBD6-C96FE0A0680F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5367A9B-02B0-4C90-B391-A0FA141A74B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{540CE9DB-4F91-4DA8-879B-A5CEB9C1B315}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>If red light is lit up the area is not clear</t>
+  </si>
+  <si>
+    <t>IR Sensor</t>
+  </si>
+  <si>
+    <t>Sends light signals to to detect obstacles. Used for rear obstacle detection</t>
   </si>
 </sst>
 </file>
@@ -640,7 +646,7 @@
   <cols>
     <col min="1" max="1" width="23.77734375" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -895,8 +901,14 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>58</v>
+      </c>
       <c r="B38" t="s">
         <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>